<commit_message>
Try to fix figures
</commit_message>
<xml_diff>
--- a/Code/HA-Models/Target_AggMPCX_LiquWealth/Data_AggMPC_LotteryWin.xlsx
+++ b/Code/HA-Models/Target_AggMPCX_LiquWealth/Data_AggMPC_LotteryWin.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -463,10 +463,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>0.5028904953788366</v>
+        <v>0.50498035816488</v>
       </c>
       <c r="D2" t="n">
-        <v>0.4865946797507227</v>
+        <v>0.4896850342321357</v>
       </c>
       <c r="E2" t="n">
         <v>0.5056845</v>
@@ -480,10 +480,10 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1774724807286316</v>
+        <v>0.1766346839572729</v>
       </c>
       <c r="D3" t="n">
-        <v>0.2420119890740031</v>
+        <v>0.2397575677814817</v>
       </c>
       <c r="E3" t="n">
         <v>0.1759051</v>
@@ -497,10 +497,10 @@
         <v>2</v>
       </c>
       <c r="C4" t="n">
-        <v>0.06883397053823591</v>
+        <v>0.06859236999288705</v>
       </c>
       <c r="D4" t="n">
-        <v>0.06585587115020564</v>
+        <v>0.06577848334310521</v>
       </c>
       <c r="E4" t="n">
         <v>0.1035106</v>
@@ -514,10 +514,10 @@
         <v>3</v>
       </c>
       <c r="C5" t="n">
-        <v>0.03308301932852964</v>
+        <v>0.03317464083868185</v>
       </c>
       <c r="D5" t="n">
-        <v>0.02839299407078133</v>
+        <v>0.02854785809170104</v>
       </c>
       <c r="E5" t="n">
         <v>0.0444222</v>
@@ -531,10 +531,10 @@
         <v>4</v>
       </c>
       <c r="C6" t="n">
-        <v>0.01915927998178294</v>
+        <v>0.0188834237645921</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01625385792084194</v>
+        <v>0.01603133985081042</v>
       </c>
       <c r="E6" t="n">
         <v>0.0336616</v>

</xml_diff>